<commit_message>
Worked on index tables - still in Test_figure_tables for Fleets 6 adn 7
</commit_message>
<xml_diff>
--- a/txt_files/Fleet5_DebWV_IndexData.xlsx
+++ b/txt_files/Fleet5_DebWV_IndexData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16035" windowHeight="6510" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16037" windowHeight="6514" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AIC" sheetId="1" r:id="rId1"/>
@@ -76,9 +76,6 @@
     <t>Remove errors, missing data</t>
   </si>
   <si>
-    <t>Remove 1987 (sampled only MNT) ,1990-1991 low sample sizes</t>
-  </si>
-  <si>
     <t>Remove reefs that never encountered GBY</t>
   </si>
   <si>
@@ -98,6 +95,9 @@
   </si>
   <si>
     <t>PositiveDrifts</t>
+  </si>
+  <si>
+    <t>Remove 1987 (sampled only MNT), 1990-1991 low sample sizes</t>
   </si>
 </sst>
 </file>
@@ -154,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -163,6 +163,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,9 +450,9 @@
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -462,7 +463,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -473,7 +474,7 @@
         <v>3330</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -484,7 +485,7 @@
         <v>2906</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -495,7 +496,7 @@
         <v>2880</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -506,7 +507,7 @@
         <v>3286</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -517,7 +518,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -528,7 +529,7 @@
         <v>2844</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -539,7 +540,7 @@
         <v>2902</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -559,91 +560,95 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="2" max="3" width="9.23046875" style="4"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C1" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>15</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="4">
         <v>6691</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="4">
         <v>1470</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="4">
+        <v>4283</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1372</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
         <v>16</v>
       </c>
-      <c r="B3">
-        <v>4283</v>
-      </c>
-      <c r="C3">
+      <c r="B4" s="4">
+        <v>4022</v>
+      </c>
+      <c r="C4" s="4">
         <v>1372</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
         <v>17</v>
       </c>
-      <c r="B4">
-        <v>4022</v>
-      </c>
-      <c r="C4">
-        <v>1372</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" s="4">
+        <v>3762</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
         <v>18</v>
       </c>
-      <c r="B5">
-        <v>3762</v>
-      </c>
-      <c r="C5">
-        <v>1300</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B6" s="4">
+        <v>3515</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1279</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
         <v>19</v>
       </c>
-      <c r="B6">
-        <v>3515</v>
-      </c>
-      <c r="C6">
-        <v>1279</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7">
+      <c r="B7" s="4">
         <v>2411</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="4">
         <v>1096</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -651,24 +656,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
         <v>21</v>
       </c>
-      <c r="C1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="1">
         <v>1988</v>
       </c>
@@ -679,7 +684,7 @@
         <v>0.16811657839449862</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
         <v>1989</v>
       </c>
@@ -690,7 +695,7 @@
         <v>0.15195743081718394</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
         <v>1992</v>
       </c>
@@ -701,7 +706,7 @@
         <v>0.16743606641307573</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
         <v>1993</v>
       </c>
@@ -712,7 +717,7 @@
         <v>0.13741858194398887</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" s="1">
         <v>1994</v>
       </c>
@@ -723,7 +728,7 @@
         <v>0.11638927952183344</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" s="1">
         <v>1995</v>
       </c>
@@ -734,7 +739,7 @@
         <v>0.10456951645290401</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" s="1">
         <v>1996</v>
       </c>
@@ -745,7 +750,7 @@
         <v>0.10371983439245235</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" s="1">
         <v>1997</v>
       </c>
@@ -756,7 +761,7 @@
         <v>9.4221415937302225E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" s="1">
         <v>1998</v>
       </c>

</xml_diff>